<commit_message>
Added literature review table
</commit_message>
<xml_diff>
--- a/literature_review/literature_review_table.xlsx
+++ b/literature_review/literature_review_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/b1017579/Documents/PhD/Reports/6. ELECSIM/Paper/literature_review/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFFA77D-8EED-F241-AAE5-C0019DD65060}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C69F70A-2864-9745-84DF-F6AAC4205CCB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" xr2:uid="{D6E4C5E8-536E-D048-A5FE-E0778643436E}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
-  <si>
-    <t>Agent based model table</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="25">
   <si>
     <t>Tool name</t>
   </si>
@@ -72,9 +69,6 @@
     <t>Bilateral</t>
   </si>
   <si>
-    <t>Stochasticity</t>
-  </si>
-  <si>
     <t>Demand</t>
   </si>
   <si>
@@ -84,7 +78,28 @@
     <t>Country Generalisability</t>
   </si>
   <si>
-    <t>Forced outages</t>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Day-ahead</t>
+  </si>
+  <si>
+    <t>EU</t>
+  </si>
+  <si>
+    <t>ElecSIM</t>
+  </si>
+  <si>
+    <t>Futures</t>
+  </si>
+  <si>
+    <t>Outages</t>
+  </si>
+  <si>
+    <t>Outages/Demand</t>
+  </si>
+  <si>
+    <t>Stochastic Inputs</t>
   </si>
 </sst>
 </file>
@@ -446,7 +461,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -462,42 +477,57 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>22</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="20" x14ac:dyDescent="0.2">
@@ -505,38 +535,59 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="F6" t="s">
-        <v>12</v>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="20" x14ac:dyDescent="0.2">
@@ -544,40 +595,83 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>